<commit_message>
fills in metadata for release tables
</commit_message>
<xml_diff>
--- a/data-raw/metadata/battle-release-metadata.xlsx
+++ b/data-raw/metadata/battle-release-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Downloads/metadata template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D68CA221-3B16-704B-A5F0-DE6707F29C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55E604A-B4F5-CC4C-9616-38904DCF2545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34220" yWindow="-19960" windowWidth="30240" windowHeight="17100" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -74,6 +74,135 @@
   </si>
   <si>
     <t>attribute_name</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>Site location</t>
+  </si>
+  <si>
+    <t>ordinal</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>date_released</t>
+  </si>
+  <si>
+    <t>Date of release</t>
+  </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>time_released</t>
+  </si>
+  <si>
+    <t>Time of release</t>
+  </si>
+  <si>
+    <t>HH:MM:SS</t>
+  </si>
+  <si>
+    <t>number_released</t>
+  </si>
+  <si>
+    <t>Number of fish released</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>count of fish</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>median_fork_length_released</t>
+  </si>
+  <si>
+    <t>Median fork length of the released fish</t>
+  </si>
+  <si>
+    <t>millimeter</t>
+  </si>
+  <si>
+    <t>release_id</t>
+  </si>
+  <si>
+    <t>Release ID (to connect to recapture table)</t>
+  </si>
+  <si>
+    <t>nominal</t>
+  </si>
+  <si>
+    <t>days_held_post_mark</t>
+  </si>
+  <si>
+    <t>How many days the fish was held post-marking</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>day_or_night_release</t>
+  </si>
+  <si>
+    <t>Whether the release was conducted at day or night, levels = c("night", "day", NA)</t>
+  </si>
+  <si>
+    <t>release_temp</t>
+  </si>
+  <si>
+    <t>Temperature recorded at release</t>
+  </si>
+  <si>
+    <t>Celsius</t>
+  </si>
+  <si>
+    <t>release_flow</t>
+  </si>
+  <si>
+    <t>Flow recorded at release</t>
+  </si>
+  <si>
+    <t>cubicFeetPerSecond</t>
+  </si>
+  <si>
+    <t>release_turbidity</t>
+  </si>
+  <si>
+    <t>Turbidity recorded at release</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>origin_released</t>
+  </si>
+  <si>
+    <t>Origin of the released fish. Levels = c("natural", "hatchery", NA)</t>
+  </si>
+  <si>
+    <t>2004-14-14</t>
+  </si>
+  <si>
+    <t>2021-03-08</t>
+  </si>
+  <si>
+    <t>02:05:00</t>
+  </si>
+  <si>
+    <t>23:23:00</t>
   </si>
 </sst>
 </file>
@@ -128,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -143,6 +272,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -231,7 +363,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -519,7 +651,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -527,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMG10"/>
+  <dimension ref="A1:AMG13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,26 +723,297 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="2"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G10" s="6"/>
+    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="5">
+        <v>65</v>
+      </c>
+      <c r="M5" s="5">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="5">
+        <v>33</v>
+      </c>
+      <c r="M6" s="5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="5">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="M10" s="5">
+        <v>62.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="5">
+        <v>202</v>
+      </c>
+      <c r="M11" s="5">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="5">
+        <v>1.57</v>
+      </c>
+      <c r="M12" s="5">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1021" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1020" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1021" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1020" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1021" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1020" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>